<commit_message>
frontend: Updating styles for the Button component
</commit_message>
<xml_diff>
--- a/ui_tests_pw/test_data/import_template_test_50_users.xlsx
+++ b/ui_tests_pw/test_data/import_template_test_50_users.xlsx
@@ -641,8 +641,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -743,7 +744,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1001,17 +1002,17 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:E51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
frontend: NavBar: Tabs were messed up when localization changed to, e.g., Spanish
</commit_message>
<xml_diff>
--- a/ui_tests_pw/test_data/import_template_test_50_users.xlsx
+++ b/ui_tests_pw/test_data/import_template_test_50_users.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">LN Watermelon 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 1</t>
+    <t xml:space="preserve">Some text for bio 1</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-2</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">LN Watermelon 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 2</t>
+    <t xml:space="preserve">Some text for bio 2</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-3</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">LN Watermelon 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 3</t>
+    <t xml:space="preserve">Some text for bio 3</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-4</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">LN Watermelon 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 4</t>
+    <t xml:space="preserve">Some text for bio 4</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-5</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">LN Watermelon 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 5</t>
+    <t xml:space="preserve">Some text for bio 5</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-6</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">LN Watermelon 6</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 6</t>
+    <t xml:space="preserve">Some text for bio 6</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-7</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">LN Watermelon 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 7</t>
+    <t xml:space="preserve">Some text for bio 7</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-8</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">LN Watermelon 8</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 8</t>
+    <t xml:space="preserve">Some text for bio 8</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-9</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">LN Watermelon 9</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 9</t>
+    <t xml:space="preserve">Some text for bio 9</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-10</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">LN Watermelon 10</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 10</t>
+    <t xml:space="preserve">Some text for bio 10</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-11</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">LN Watermelon 11</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 11</t>
+    <t xml:space="preserve">Some text for bio 11</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-12</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">LN Watermelon 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 12</t>
+    <t xml:space="preserve">Some text for bio 12</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-13</t>
@@ -190,7 +190,7 @@
     <t xml:space="preserve">LN Watermelon 13</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 13</t>
+    <t xml:space="preserve">Some text for bio 13</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-14</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">LN Watermelon 14</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 14</t>
+    <t xml:space="preserve">Some text for bio 14</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-15</t>
@@ -214,7 +214,7 @@
     <t xml:space="preserve">LN Watermelon 15</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 15</t>
+    <t xml:space="preserve">Some text for bio 15</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-16</t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">LN Watermelon 16</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 16</t>
+    <t xml:space="preserve">Some text for bio 16</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-17</t>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">LN Watermelon 17</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 17</t>
+    <t xml:space="preserve">Some text for bio 17</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-18</t>
@@ -250,7 +250,7 @@
     <t xml:space="preserve">LN Watermelon 18</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 18</t>
+    <t xml:space="preserve">Some text for bio 18</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-19</t>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">LN Watermelon 19</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 19</t>
+    <t xml:space="preserve">Some text for bio 19</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-20</t>
@@ -274,7 +274,7 @@
     <t xml:space="preserve">LN Watermelon 20</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 20</t>
+    <t xml:space="preserve">Some text for bio 20</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-21</t>
@@ -286,7 +286,7 @@
     <t xml:space="preserve">LN Watermelon 21</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 21</t>
+    <t xml:space="preserve">Some text for bio 21</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-22</t>
@@ -298,7 +298,7 @@
     <t xml:space="preserve">LN Watermelon 22</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 22</t>
+    <t xml:space="preserve">Some text for bio 22</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-23</t>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">LN Watermelon 23</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 23</t>
+    <t xml:space="preserve">Some text for bio 23</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-24</t>
@@ -322,7 +322,7 @@
     <t xml:space="preserve">LN Watermelon 24</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 24</t>
+    <t xml:space="preserve">Some text for bio 24</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-25</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">LN Watermelon 25</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 25</t>
+    <t xml:space="preserve">Some text for bio 25</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-26</t>
@@ -346,7 +346,7 @@
     <t xml:space="preserve">LN Watermelon 26</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 26</t>
+    <t xml:space="preserve">Some text for bio 26</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-27</t>
@@ -358,7 +358,7 @@
     <t xml:space="preserve">LN Watermelon 27</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 27</t>
+    <t xml:space="preserve">Some text for bio 27</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-28</t>
@@ -370,7 +370,7 @@
     <t xml:space="preserve">LN Watermelon 28</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 28</t>
+    <t xml:space="preserve">Some text for bio 28</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-29</t>
@@ -382,7 +382,7 @@
     <t xml:space="preserve">LN Watermelon 29</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 29</t>
+    <t xml:space="preserve">Some text for bio 29</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-30</t>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">LN Watermelon 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 30</t>
+    <t xml:space="preserve">Some text for bio 30</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-31</t>
@@ -406,7 +406,7 @@
     <t xml:space="preserve">LN Watermelon 31</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 31</t>
+    <t xml:space="preserve">Some text for bio 31</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-32</t>
@@ -418,7 +418,7 @@
     <t xml:space="preserve">LN Watermelon 32</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 32</t>
+    <t xml:space="preserve">Some text for bio 32</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-33</t>
@@ -430,7 +430,7 @@
     <t xml:space="preserve">LN Watermelon 33</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 33</t>
+    <t xml:space="preserve">Some text for bio 33</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-34</t>
@@ -442,7 +442,7 @@
     <t xml:space="preserve">LN Watermelon 34</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 34</t>
+    <t xml:space="preserve">Some text for bio 34</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-35</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">LN Watermelon 35</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 35</t>
+    <t xml:space="preserve">Some text for bio 35</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-36</t>
@@ -466,7 +466,7 @@
     <t xml:space="preserve">LN Watermelon 36</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 36</t>
+    <t xml:space="preserve">Some text for bio 36</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-37</t>
@@ -478,7 +478,7 @@
     <t xml:space="preserve">LN Watermelon 37</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 37</t>
+    <t xml:space="preserve">Some text for bio 37</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-38</t>
@@ -490,7 +490,7 @@
     <t xml:space="preserve">LN Watermelon 38</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 38</t>
+    <t xml:space="preserve">Some text for bio 38</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-39</t>
@@ -502,7 +502,7 @@
     <t xml:space="preserve">LN Watermelon 39</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 39</t>
+    <t xml:space="preserve">Some text for bio 39</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-40</t>
@@ -514,7 +514,7 @@
     <t xml:space="preserve">LN Watermelon 40</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 40</t>
+    <t xml:space="preserve">Some text for bio 40</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-41</t>
@@ -526,7 +526,7 @@
     <t xml:space="preserve">LN Watermelon 41</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 41</t>
+    <t xml:space="preserve">Some text for bio 41</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-42</t>
@@ -538,7 +538,7 @@
     <t xml:space="preserve">LN Watermelon 42</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 42</t>
+    <t xml:space="preserve">Some text for bio 42</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-43</t>
@@ -550,7 +550,7 @@
     <t xml:space="preserve">LN Watermelon 43</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 43</t>
+    <t xml:space="preserve">Some text for bio 43</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-44</t>
@@ -562,7 +562,7 @@
     <t xml:space="preserve">LN Watermelon 44</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 44</t>
+    <t xml:space="preserve">Some text for bio 44</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-45</t>
@@ -574,7 +574,7 @@
     <t xml:space="preserve">LN Watermelon 45</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 45</t>
+    <t xml:space="preserve">Some text for bio 45</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-46</t>
@@ -586,7 +586,7 @@
     <t xml:space="preserve">LN Watermelon 46</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 46</t>
+    <t xml:space="preserve">Some text for bio 46</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-47</t>
@@ -598,7 +598,7 @@
     <t xml:space="preserve">LN Watermelon 47</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 47</t>
+    <t xml:space="preserve">Some text for bio 47</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-48</t>
@@ -610,7 +610,7 @@
     <t xml:space="preserve">LN Watermelon 48</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 48</t>
+    <t xml:space="preserve">Some text for bio 48</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-49</t>
@@ -622,7 +622,7 @@
     <t xml:space="preserve">LN Watermelon 49</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 49</t>
+    <t xml:space="preserve">Some text for bio 49</t>
   </si>
   <si>
     <t xml:space="preserve">ui-test-watermelon-50</t>
@@ -634,7 +634,7 @@
     <t xml:space="preserve">LN Watermelon 50</t>
   </si>
   <si>
-    <t xml:space="preserve">Bio 50</t>
+    <t xml:space="preserve">Some text for bio 50</t>
   </si>
 </sst>
 </file>

</xml_diff>